<commit_message>
Changed examples to match new update, spacing
</commit_message>
<xml_diff>
--- a/basic-insurer-dashboard/example reports/claims-report-as-of-2019-06-20.xlsx
+++ b/basic-insurer-dashboard/example reports/claims-report-as-of-2019-06-20.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t xml:space="preserve">Example Client Name</t>
   </si>
@@ -25,7 +25,7 @@
     <t xml:space="preserve">Evaluated as of June 20, 2019</t>
   </si>
   <si>
-    <t xml:space="preserve">Report GeneratedJune 20, 2019</t>
+    <t xml:space="preserve">Report Generated June 20, 2019</t>
   </si>
   <si>
     <t xml:space="preserve">Workers' Compensation Claims Report</t>
@@ -103,58 +103,40 @@
     <t xml:space="preserve">Status</t>
   </si>
   <si>
-    <t xml:space="preserve">claim-661</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shovein, Erin</t>
+    <t xml:space="preserve">claim-663</t>
+  </si>
+  <si>
+    <t xml:space="preserve">el-Shahin, Raaid</t>
   </si>
   <si>
     <t xml:space="preserve">CA</t>
   </si>
   <si>
-    <t xml:space="preserve">claim-187</t>
-  </si>
-  <si>
-    <t xml:space="preserve">al-Barakat, Ghaidaa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">claim-526</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Montenegro, Ethan</t>
-  </si>
-  <si>
     <t xml:space="preserve">Closed</t>
   </si>
   <si>
-    <t xml:space="preserve">claim-685</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leon, Sky</t>
-  </si>
-  <si>
-    <t xml:space="preserve">claim-205</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Robinson, Jazmine</t>
+    <t xml:space="preserve">claim-328</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moore, Anthony</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">claim-997</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melling, Kayla</t>
   </si>
   <si>
     <t xml:space="preserve">TX</t>
   </si>
   <si>
-    <t xml:space="preserve">claim-220</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mclaughlin, Shaquoya</t>
-  </si>
-  <si>
-    <t xml:space="preserve">claim-800</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deveyra, Lohitha</t>
+    <t xml:space="preserve">claim-382</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fischer, Zandra</t>
   </si>
   <si>
     <t xml:space="preserve">Loss &amp; ALAE</t>
@@ -211,6 +193,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <b/>
       <u val="single"/>
     </font>
   </fonts>
@@ -274,7 +257,7 @@
       <xdr:row xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">0</xdr:row>
       <xdr:rowOff xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" cx="4270248" cy="1143000"/>
+    <xdr:ext xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" cx="4572000" cy="1143000"/>
     <xdr:pic xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
       <xdr:nvPicPr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
         <xdr:cNvPr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" id="1" name="Picture 1"/>
@@ -656,10 +639,10 @@
     </row>
     <row r="8">
       <c r="B8" s="6" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9">
@@ -687,19 +670,19 @@
         <v>15</v>
       </c>
       <c r="B10" s="7" t="n">
-        <v>6601418</v>
+        <v>8062709</v>
       </c>
       <c r="C10" s="7" t="n">
         <v>0</v>
       </c>
       <c r="D10" s="7" t="n">
-        <v>6601418</v>
+        <v>8062709</v>
       </c>
       <c r="E10" s="7" t="n">
         <v>0</v>
       </c>
       <c r="F10" s="7" t="n">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11">
@@ -707,19 +690,19 @@
         <v>16</v>
       </c>
       <c r="B11" s="7" t="n">
-        <v>7532424</v>
+        <v>11153815</v>
       </c>
       <c r="C11" s="7" t="n">
-        <v>0</v>
+        <v>21392</v>
       </c>
       <c r="D11" s="7" t="n">
-        <v>7532424</v>
+        <v>11175207</v>
       </c>
       <c r="E11" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="7" t="n">
-        <v>135</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12">
@@ -727,19 +710,19 @@
         <v>17</v>
       </c>
       <c r="B12" s="7" t="n">
-        <v>6644795</v>
+        <v>7938500</v>
       </c>
       <c r="C12" s="7" t="n">
-        <v>5069</v>
+        <v>0</v>
       </c>
       <c r="D12" s="7" t="n">
-        <v>6649864</v>
+        <v>7938500</v>
       </c>
       <c r="E12" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" s="7" t="n">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13">
@@ -747,19 +730,19 @@
         <v>18</v>
       </c>
       <c r="B13" s="7" t="n">
-        <v>6384523</v>
+        <v>6346917</v>
       </c>
       <c r="C13" s="7" t="n">
-        <v>189893</v>
+        <v>86050</v>
       </c>
       <c r="D13" s="7" t="n">
-        <v>6574416</v>
+        <v>6432967</v>
       </c>
       <c r="E13" s="7" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F13" s="7" t="n">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14">
@@ -767,19 +750,19 @@
         <v>19</v>
       </c>
       <c r="B14" s="7" t="n">
-        <v>7515235</v>
+        <v>4584134</v>
       </c>
       <c r="C14" s="7" t="n">
-        <v>332026</v>
+        <v>296425</v>
       </c>
       <c r="D14" s="7" t="n">
-        <v>7847261</v>
+        <v>4880559</v>
       </c>
       <c r="E14" s="7" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F14" s="7" t="n">
-        <v>152</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15">
@@ -787,19 +770,19 @@
         <v>20</v>
       </c>
       <c r="B15" s="7" t="n">
-        <v>6261986</v>
+        <v>5169959</v>
       </c>
       <c r="C15" s="7" t="n">
-        <v>1019692</v>
+        <v>1007062</v>
       </c>
       <c r="D15" s="7" t="n">
-        <v>7281678</v>
+        <v>6177021</v>
       </c>
       <c r="E15" s="7" t="n">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F15" s="7" t="n">
-        <v>135</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16">
@@ -807,19 +790,19 @@
         <v>21</v>
       </c>
       <c r="B16" s="7" t="n">
-        <v>3966270</v>
+        <v>2756407</v>
       </c>
       <c r="C16" s="7" t="n">
-        <v>2192489</v>
+        <v>2135840</v>
       </c>
       <c r="D16" s="7" t="n">
-        <v>6158759</v>
+        <v>4892247</v>
       </c>
       <c r="E16" s="7" t="n">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="F16" s="7" t="n">
-        <v>140</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17">
@@ -827,19 +810,19 @@
         <v>22</v>
       </c>
       <c r="B17" s="7" t="n">
-        <v>337068</v>
+        <v>604945</v>
       </c>
       <c r="C17" s="7" t="n">
-        <v>523367</v>
+        <v>947565</v>
       </c>
       <c r="D17" s="7" t="n">
-        <v>860435</v>
+        <v>1552510</v>
       </c>
       <c r="E17" s="7" t="n">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="F17" s="7" t="n">
-        <v>26</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18">
@@ -855,19 +838,19 @@
         <v>23</v>
       </c>
       <c r="B19" s="7" t="n">
-        <v>45243719</v>
+        <v>46617386</v>
       </c>
       <c r="C19" s="7" t="n">
-        <v>4262536</v>
+        <v>4494334</v>
       </c>
       <c r="D19" s="7" t="n">
-        <v>49506255</v>
+        <v>51111720</v>
       </c>
       <c r="E19" s="7" t="n">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="F19" s="7" t="n">
-        <v>1000</v>
+        <v>997</v>
       </c>
     </row>
   </sheetData>
@@ -929,13 +912,13 @@
     </row>
     <row r="8">
       <c r="F8" s="6" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9">
@@ -978,7 +961,7 @@
         <v>29</v>
       </c>
       <c r="B10" s="5" t="n">
-        <v>42511</v>
+        <v>42229</v>
       </c>
       <c r="C10" t="s">
         <v>30</v>
@@ -987,243 +970,175 @@
         <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="F10" s="7" t="n">
-        <v>180048</v>
+        <v>302907</v>
       </c>
       <c r="G10" s="7" t="n">
-        <v>187619</v>
+        <v>302907</v>
       </c>
       <c r="H10" s="7" t="n">
-        <v>16421</v>
+        <v>70257</v>
       </c>
       <c r="I10" s="7" t="n">
-        <v>24235</v>
+        <v>70757</v>
       </c>
       <c r="J10" s="7" t="n">
-        <v>163627</v>
+        <v>232650</v>
       </c>
       <c r="K10" s="7" t="n">
-        <v>163384</v>
+        <v>232150</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="5" t="n">
+        <v>42871</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="5" t="n">
-        <v>43101</v>
-      </c>
-      <c r="C11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" t="s">
-        <v>14</v>
-      </c>
       <c r="F11" s="7" t="n">
-        <v>176961</v>
+        <v>218903</v>
       </c>
       <c r="G11" s="7" t="n">
-        <v>177461</v>
+        <v>218903</v>
       </c>
       <c r="H11" s="7" t="n">
-        <v>13450</v>
+        <v>68156</v>
       </c>
       <c r="I11" s="7" t="n">
-        <v>32976</v>
+        <v>86522</v>
       </c>
       <c r="J11" s="7" t="n">
-        <v>163511</v>
+        <v>150747</v>
       </c>
       <c r="K11" s="7" t="n">
-        <v>144485</v>
+        <v>132381</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B12" s="5" t="n">
-        <v>43010</v>
+        <v>43107</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E12" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F12" s="7" t="n">
-        <v>148200</v>
+        <v>126598</v>
       </c>
       <c r="G12" s="7" t="n">
-        <v>148200</v>
+        <v>126598</v>
       </c>
       <c r="H12" s="7" t="n">
-        <v>9286</v>
+        <v>2613</v>
       </c>
       <c r="I12" s="7" t="n">
-        <v>9786</v>
+        <v>4026</v>
       </c>
       <c r="J12" s="7" t="n">
-        <v>138914</v>
+        <v>123985</v>
       </c>
       <c r="K12" s="7" t="n">
-        <v>138414</v>
+        <v>122572</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B13" s="5" t="n">
-        <v>43071</v>
+        <v>42954</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E13" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="F13" s="7" t="n">
-        <v>176557</v>
+        <v>127462</v>
       </c>
       <c r="G13" s="7" t="n">
-        <v>265458</v>
+        <v>127462</v>
       </c>
       <c r="H13" s="7" t="n">
-        <v>47258</v>
+        <v>5303</v>
       </c>
       <c r="I13" s="7" t="n">
-        <v>127464</v>
+        <v>6359</v>
       </c>
       <c r="J13" s="7" t="n">
-        <v>129299</v>
+        <v>122159</v>
       </c>
       <c r="K13" s="7" t="n">
-        <v>137994</v>
+        <v>121103</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="5" t="n">
-        <v>42280</v>
-      </c>
-      <c r="C14" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="7" t="n">
-        <v>191697</v>
-      </c>
-      <c r="G14" s="7" t="n">
-        <v>196275</v>
-      </c>
-      <c r="H14" s="7" t="n">
-        <v>68166</v>
-      </c>
-      <c r="I14" s="7" t="n">
-        <v>74409</v>
-      </c>
-      <c r="J14" s="7" t="n">
-        <v>123531</v>
-      </c>
-      <c r="K14" s="7" t="n">
-        <v>121866</v>
-      </c>
+      <c r="A14" s="8"/>
+      <c r="B14" s="5"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
     </row>
     <row r="15">
       <c r="A15" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" s="5" t="n">
-        <v>43124</v>
-      </c>
-      <c r="C15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="7" t="n">
-        <v>115055</v>
-      </c>
-      <c r="G15" s="7" t="n">
-        <v>115555</v>
-      </c>
-      <c r="H15" s="7" t="n">
-        <v>9723</v>
-      </c>
-      <c r="I15" s="7" t="n">
-        <v>10223</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
       <c r="J15" s="7" t="n">
-        <v>105332</v>
+        <v>629541</v>
       </c>
       <c r="K15" s="7" t="n">
-        <v>105332</v>
+        <v>608206</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" s="5" t="n">
-        <v>43161</v>
-      </c>
-      <c r="C16" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="7" t="n">
-        <v>116002</v>
-      </c>
-      <c r="G16" s="7" t="n">
-        <v>126590</v>
-      </c>
-      <c r="H16" s="7" t="n">
-        <v>13873</v>
-      </c>
-      <c r="I16" s="7" t="n">
-        <v>21881</v>
-      </c>
-      <c r="J16" s="7" t="n">
-        <v>102129</v>
-      </c>
-      <c r="K16" s="7" t="n">
-        <v>104709</v>
-      </c>
+      <c r="A16" s="8"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
     </row>
     <row r="17">
       <c r="A17" s="8"/>
-      <c r="B17" s="5"/>
-      <c r="C17"/>
-      <c r="D17"/>
-      <c r="E17"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
@@ -1232,23 +1147,13 @@
       <c r="K17" s="7"/>
     </row>
     <row r="18">
-      <c r="A18" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="5"/>
-      <c r="C18"/>
-      <c r="D18"/>
-      <c r="E18"/>
+      <c r="A18" s="8"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
-      <c r="J18" s="7" t="n">
-        <v>926343</v>
-      </c>
-      <c r="K18" s="7" t="n">
-        <v>916184</v>
-      </c>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
     </row>
     <row r="19">
       <c r="A19" s="8"/>

</xml_diff>